<commit_message>
Used matplotlib to graph simple excel file created from dummy data.
</commit_message>
<xml_diff>
--- a/Python-Linux/Testing/test.xlsx
+++ b/Python-Linux/Testing/test.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,10 +436,20 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>Unnamed: 0</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>NAME</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
           <t>WIDTH</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>HEIGHT</t>
         </is>
@@ -450,9 +460,17 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>James</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
         <v>22</v>
       </c>
-      <c r="C2" t="n">
+      <c r="E2" t="n">
         <v>22</v>
       </c>
     </row>
@@ -461,9 +479,17 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Timmy</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
         <v>12</v>
       </c>
-      <c r="C3" t="n">
+      <c r="E3" t="n">
         <v>45</v>
       </c>
     </row>
@@ -472,10 +498,35 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
+        <v>2</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Sally</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
         <v>12</v>
       </c>
-      <c r="C4" t="n">
+      <c r="E4" t="n">
         <v>43</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr"/>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Andrew</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>20</v>
+      </c>
+      <c r="E5" t="n">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>